<commit_message>
Alleen nog constraint 8
Co-authored-by: lynnvorgers <lynnvorgers@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Problem 1 - Data/airport_data.xlsx
+++ b/Problem 1 - Data/airport_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thijm\OneDrive\Documents\MSc Aerospace Engineering\Airline Planning &amp; Optimisation\ASSIGNMENT 1\Airline_planning\Problem 1 - Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aadb9d128a4cfa1d/Documenten/python/Airline_planning/Problem 1 - Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFC3E91-61D6-4436-823A-96C40EF56D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9EFC3E91-61D6-4436-823A-96C40EF56D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E28E4A54-DC89-4472-B4D4-E6B4CA2CFB24}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1035" windowWidth="13830" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,12 +483,15 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +553,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -615,7 +618,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -680,7 +683,7 @@
         <v>32.697899999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -745,7 +748,7 @@
         <v>-16.7745</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -810,7 +813,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>

</xml_diff>